<commit_message>
Add signal-configs support for gd32f350
</commit_message>
<xml_diff>
--- a/data/GD32F350 alternate functions summary.xlsx
+++ b/data/GD32F350 alternate functions summary.xlsx
@@ -1178,7 +1178,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">SPI  _MISO</t>
+      <t xml:space="preserve">SPI1_MISO</t>
     </r>
     <r>
       <rPr>
@@ -1228,7 +1228,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">SPI  _MOSI</t>
+      <t xml:space="preserve">SPI1_MOSI</t>
     </r>
     <r>
       <rPr>
@@ -1725,8 +1725,8 @@
   </sheetPr>
   <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1739,7 +1739,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="8.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="6.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="6.64"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="2" width="8.73"/>
   </cols>
   <sheetData>
@@ -2448,7 +2448,7 @@
       <c r="H31" s="5"/>
       <c r="I31" s="7"/>
     </row>
-    <row r="32" customFormat="false" ht="28.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="35.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
         <v>147</v>
       </c>
@@ -2469,7 +2469,7 @@
       <c r="H32" s="5"/>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" customFormat="false" ht="32.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="35.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
         <v>151</v>
       </c>

</xml_diff>